<commit_message>
Update performance results for comparison between H5Dwrite and H5Dwrite_multi
Former-commit-id: 0ea8c595db816d7255cbac1669ed0411edc9f481
</commit_message>
<xml_diff>
--- a/RFCs/HDF5_Library/HPC_H5Dread_multi_H5Dwrite_multi/H5Dwrite_multi_Perfrom_v1.xlsx
+++ b/RFCs/HDF5_Library/HPC_H5Dread_multi_H5Dwrite_multi/H5Dwrite_multi_Perfrom_v1.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="0" windowWidth="25605" windowHeight="14925" tabRatio="500"/>
+    <workbookView xWindow="6420" yWindow="1080" windowWidth="25605" windowHeight="14925" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -21,26 +24,26 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
-    <t># of chunked dsets</t>
-  </si>
-  <si>
-    <t># of contig dsets</t>
-  </si>
-  <si>
     <t>H5Dwrite (sec)</t>
   </si>
   <si>
     <t>H5Dwrite_multi (sec)</t>
   </si>
   <si>
-    <t>NOTE: this test was perfromed on wallaby</t>
+    <t>Perfromance Comparison between H5Dwrite_multi and H5Dwrite on Wallaby</t>
+  </si>
+  <si>
+    <t># of CHUNKED dsets</t>
+  </si>
+  <si>
+    <t># of CONTIG dsets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,6 +74,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -80,12 +91,109 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -100,12 +208,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -166,7 +285,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>[1]Sheet1!$A$111:$A$115</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -190,7 +309,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$9</c:f>
+              <c:f>[1]Sheet1!$B$111:$B$115</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -232,7 +351,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:f>[1]Sheet1!$A$111:$A$115</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -256,7 +375,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$9</c:f>
+              <c:f>[1]Sheet1!$C$111:$C$115</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -290,11 +409,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119964416"/>
-        <c:axId val="119966336"/>
+        <c:axId val="88098688"/>
+        <c:axId val="88100864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119964416"/>
+        <c:axId val="88098688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -323,7 +442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119966336"/>
+        <c:crossAx val="88100864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -331,7 +450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119966336"/>
+        <c:axId val="88100864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,7 +485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119964416"/>
+        <c:crossAx val="88098688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -429,7 +548,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$10</c:f>
+              <c:f>[1]Sheet1!$E$111:$E$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -453,7 +572,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$5:$F$9</c:f>
+              <c:f>[1]Sheet1!$F$111:$F$115</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -488,7 +607,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$10</c:f>
+              <c:f>[1]Sheet1!$E$111:$E$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -512,7 +631,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$5:$G$9</c:f>
+              <c:f>[1]Sheet1!$G$111:$G$115</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -546,11 +665,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119983488"/>
-        <c:axId val="122889728"/>
+        <c:axId val="88216704"/>
+        <c:axId val="88218624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119983488"/>
+        <c:axId val="88216704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,7 +698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122889728"/>
+        <c:crossAx val="88218624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -587,7 +706,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122889728"/>
+        <c:axId val="88218624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,7 +736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119983488"/>
+        <c:crossAx val="88216704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -656,8 +775,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -686,8 +807,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 12"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -702,6 +825,120 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="111">
+          <cell r="A111">
+            <v>50</v>
+          </cell>
+          <cell r="B111">
+            <v>0.55500000000000005</v>
+          </cell>
+          <cell r="C111">
+            <v>7.5999999999999998E-2</v>
+          </cell>
+          <cell r="E111">
+            <v>400</v>
+          </cell>
+          <cell r="F111">
+            <v>0.45600000000000002</v>
+          </cell>
+          <cell r="G111">
+            <v>0.111</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="A112">
+            <v>100</v>
+          </cell>
+          <cell r="B112">
+            <v>1.077</v>
+          </cell>
+          <cell r="C112">
+            <v>4.5999999999999999E-2</v>
+          </cell>
+          <cell r="E112">
+            <v>800</v>
+          </cell>
+          <cell r="F112">
+            <v>0.90100000000000002</v>
+          </cell>
+          <cell r="G112">
+            <v>5.0999999999999997E-2</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="A113">
+            <v>200</v>
+          </cell>
+          <cell r="B113">
+            <v>2.1030000000000002</v>
+          </cell>
+          <cell r="C113">
+            <v>0.14299999999999999</v>
+          </cell>
+          <cell r="E113">
+            <v>1600</v>
+          </cell>
+          <cell r="F113">
+            <v>1.7729999999999999</v>
+          </cell>
+          <cell r="G113">
+            <v>9.8000000000000004E-2</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="A114">
+            <v>400</v>
+          </cell>
+          <cell r="B114">
+            <v>4.2460000000000004</v>
+          </cell>
+          <cell r="C114">
+            <v>0.29099999999999998</v>
+          </cell>
+          <cell r="E114">
+            <v>3200</v>
+          </cell>
+          <cell r="F114">
+            <v>3.4249999999999998</v>
+          </cell>
+          <cell r="G114">
+            <v>0.17599999999999999</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="A115">
+            <v>800</v>
+          </cell>
+          <cell r="B115">
+            <v>8.34</v>
+          </cell>
+          <cell r="C115">
+            <v>1.018</v>
+          </cell>
+          <cell r="E115">
+            <v>6400</v>
+          </cell>
+          <cell r="F115">
+            <v>7.7039999999999997</v>
+          </cell>
+          <cell r="G115">
+            <v>0.63200000000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1026,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1043,128 +1280,136 @@
     <col min="7" max="7" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:8" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>50</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="C5" s="8">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>400</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="C5">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="E5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>100</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1.077</v>
+      </c>
+      <c r="C6" s="8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>800</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="G6" s="8">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>200</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2.1030000000000002</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1600</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1.7729999999999999</v>
+      </c>
+      <c r="G7" s="8">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>400</v>
       </c>
-      <c r="F5">
-        <v>0.45600000000000002</v>
-      </c>
-      <c r="G5">
-        <v>0.111</v>
+      <c r="B8" s="9">
+        <v>4.2460000000000004</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3200</v>
+      </c>
+      <c r="F8" s="7">
+        <v>3.4249999999999998</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.17599999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>100</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.077</v>
-      </c>
-      <c r="C6">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="E6">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
         <v>800</v>
       </c>
-      <c r="F6">
-        <v>0.90100000000000002</v>
-      </c>
-      <c r="G6">
-        <v>5.0999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>200</v>
-      </c>
-      <c r="B7">
-        <v>2.1030000000000002</v>
-      </c>
-      <c r="C7">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="E7">
-        <v>1600</v>
-      </c>
-      <c r="F7">
-        <v>1.7729999999999999</v>
-      </c>
-      <c r="G7">
-        <v>9.8000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>400</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4.2460000000000004</v>
-      </c>
-      <c r="C8">
-        <v>0.29099999999999998</v>
-      </c>
-      <c r="E8">
-        <v>3200</v>
-      </c>
-      <c r="F8">
-        <v>3.4249999999999998</v>
-      </c>
-      <c r="G8">
-        <v>0.17599999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>800</v>
-      </c>
-      <c r="B9">
+      <c r="B9" s="11">
         <v>8.34</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="12">
         <v>1.018</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="10">
         <v>6400</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="13">
         <v>7.7039999999999997</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="12">
         <v>0.63200000000000001</v>
       </c>
     </row>

</xml_diff>